<commit_message>
Chorus, various aurics, archangel shield
</commit_message>
<xml_diff>
--- a/CardStats.xlsx
+++ b/CardStats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="18680" windowHeight="7400"/>
+    <workbookView activeTab="0" windowWidth="18680" windowHeight="7430"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
   <dimension ref="A1:XFD20"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="145" tabSelected="1">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -352,7 +352,7 @@
         <v>12</v>
       </c>
       <c r="E8">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
@@ -369,7 +369,7 @@
         <v>18</v>
       </c>
       <c r="K8">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:16384">
@@ -386,7 +386,7 @@
         <v>43</v>
       </c>
       <c r="E9">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
@@ -403,7 +403,7 @@
         <v>36</v>
       </c>
       <c r="K9">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:16384">
@@ -420,7 +420,7 @@
         <v>11</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G10" s="5" t="inlineStr">
         <is>
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
       </c>
       <c r="K11">
         <f>SUM(K7:K10)</f>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:16384">
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16384">
@@ -507,7 +507,7 @@
       </c>
       <c r="E13">
         <f>SUM(E7:E12)</f>
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:16384" customHeight="1" ht="15">
@@ -564,7 +564,7 @@
         <v>24</v>
       </c>
       <c r="K17">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:16384">
@@ -583,7 +583,7 @@
         <v>37</v>
       </c>
       <c r="K18">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:16384">
@@ -602,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="K19">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:16384">
@@ -620,7 +620,7 @@
       </c>
       <c r="K20">
         <f>SUM(K17:K19)</f>
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>